<commit_message>
previews de reportes terminados
pendiente el mantenimiento de áreas
</commit_message>
<xml_diff>
--- a/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
+++ b/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
@@ -48,6 +48,12 @@
   </x:si>
   <x:si>
     <x:t>1.- Materiales y suministros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FILLER DE 0.0040 A 0.009 25 HOJAS X 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FILLER DE 0.050 A 1.000  20 HOJAS X 12</x:t>
   </x:si>
   <x:si>
     <x:t>2.- Servicios</x:t>
@@ -524,15 +530,37 @@
       <x:c r="B12" t="s">
         <x:v>11</x:v>
       </x:c>
+      <x:c r="C12" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D12" t="n">
+        <x:v>58.98</x:v>
+      </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="B13" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C13" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D13" t="n">
+        <x:v>81.42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14">
+      <x:c r="B14" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15">
+      <x:c r="B15" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C15" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D13" t="n">
+      <x:c r="D15" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
cambios actualizados ult entrega
</commit_message>
<xml_diff>
--- a/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
+++ b/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>ORGANISMOS DIRECCION EJECUTIVA</x:t>
   </x:si>
@@ -29,9 +29,6 @@
     <x:t>PRESUPUESTO  DE  INVERSIONES 2017 -    FORMULACION 2017</x:t>
   </x:si>
   <x:si>
-    <x:t>(En Nuevos Soles)</x:t>
-  </x:si>
-  <x:si>
     <x:t>RUBRO</x:t>
   </x:si>
   <x:si>
@@ -41,6 +38,15 @@
     <x:t>TOTAL</x:t>
   </x:si>
   <x:si>
+    <x:t>(En Soles)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CENTRO COSTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P/U</x:t>
+  </x:si>
+  <x:si>
     <x:t>Presup 7</x:t>
   </x:si>
   <x:si>
@@ -59,7 +65,16 @@
     <x:t>1.1.1.- EQUIPAMIENTO E IMPLEMENTACION </x:t>
   </x:si>
   <x:si>
-    <x:t>HOJA DE SIERRA DE  2"     X 24" X  6 DIENTES</x:t>
+    <x:t>0503280508 - HOJA DE SIERRA DE  2"     X 24" X  6 DIENTES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400145</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5505082513 - VALVULA COMPUERTA BRONCE 1.1/4 X 125 LBS P/R</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400716</x:t>
   </x:si>
   <x:si>
     <x:t>1.2.- GASTOS DE CAPITAL NO LIGADOS A PROYECTOS DE INVERSIÓN</x:t>
@@ -74,9 +89,15 @@
     <x:t>1.2.1.1.1.- HARDWARE</x:t>
   </x:si>
   <x:si>
+    <x:t>ti</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.1.2.- SOFTWARE</x:t>
   </x:si>
   <x:si>
+    <x:t>1.2.1.1.2.- desarrollo</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.1.3.- SEGURIDAD DE LA INFORMACIÓN</x:t>
   </x:si>
   <x:si>
@@ -98,6 +119,9 @@
     <x:t>1.2.1.2.2.1.- DESARROLLO</x:t>
   </x:si>
   <x:si>
+    <x:t>0341281723 - SOFTWARE SWREUSER V.2.0</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.2.2.2.- DISEÑO</x:t>
   </x:si>
   <x:si>
@@ -116,12 +140,21 @@
     <x:t>1.2.1.3.1.- ADQUISICIÓN EQUIPOS</x:t>
   </x:si>
   <x:si>
+    <x:t>6601011730 - VENTILADOR DE PEDESTAL OSCILANTE</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.3.2.- REPOSICIÓN MOBILIARIO</x:t>
   </x:si>
   <x:si>
+    <x:t>7460071317 - ESCRITORIO EN MELAMINE EN L DE 1.50 X 1.50 MT GRAFITO C/NEGRO</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.3.3.- OTROS</x:t>
   </x:si>
   <x:si>
+    <x:t>6805131381 - CARRETILLA HIDRAULICA DE 2 TN CAPACIDAD</x:t>
+  </x:si>
+  <x:si>
     <x:t>1.2.1.4.- INFRAESTRUCTURA</x:t>
   </x:si>
   <x:si>
@@ -158,7 +191,25 @@
     <x:t>1.2.3.3.- SERVICIOS GESTIÓN INTEGRADA</x:t>
   </x:si>
   <x:si>
+    <x:t>Total Materiales</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5150.39</x:t>
+  </x:si>
+  <x:si>
     <x:t>2.- Servicios</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SR50343033 - MANIOBRA DE DESMONT. MOTOR PRINCP SALA MAQUNA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Servicios</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -190,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,13 +273,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -239,9 +325,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,301 +627,473 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:dimension ref="B2:D10"/>
+  <x:dimension ref="B2:F10"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C12" sqref="C12"/>
+      <x:selection activeCell="C13" sqref="C13"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="2" max="2" width="62.85546875" customWidth="1"/>
-    <x:col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <x:col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <x:col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <x:col min="5" max="5" width="11.42578125" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B2" s="2" t="s">
+    <x:row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B2" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C2" s="2"/>
-      <x:c r="D2" s="2"/>
-    </x:row>
-    <x:row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B3" s="2" t="s">
+      <x:c r="C2" s="5"/>
+      <x:c r="D2" s="5"/>
+      <x:c r="E2" s="5"/>
+      <x:c r="F2" s="5"/>
+    </x:row>
+    <x:row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B3" s="5" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B3 " t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="5"/>
+      <x:c r="D3" s="5"/>
+      <x:c r="E3" s="5"/>
+      <x:c r="F3" s="5"/>
+    </x:row>
+    <x:row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B4" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C4" s="5"/>
+      <x:c r="D4" s="5"/>
+      <x:c r="E4" s="5"/>
+      <x:c r="F4" s="5"/>
+    </x:row>
+    <x:row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B5" s="6"/>
+      <x:c r="C5" s="6"/>
+      <x:c r="D5" s="6"/>
+      <x:c r="E5" s="6"/>
+      <x:c r="F5" s="6"/>
+    </x:row>
+    <x:row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B6" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C6" s="2"/>
+      <x:c r="D6" s="2"/>
+      <x:c r="E6" s="2"/>
+      <x:c r="F6" s="2"/>
+    </x:row>
+    <x:row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B7" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C7" s="2"/>
+      <x:c r="D7" s="2"/>
+      <x:c r="E7" s="2"/>
+      <x:c r="F7" s="2"/>
+    </x:row>
+    <x:row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B8" s="7"/>
+      <x:c r="C8" s="7"/>
+      <x:c r="D8" s="7"/>
+      <x:c r="E8" s="7"/>
+      <x:c r="F8" s="7"/>
+    </x:row>
+    <x:row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B9" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C9" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D9" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E9" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C3" s="2"/>
-      <x:c r="D3" s="2"/>
-    </x:row>
-    <x:row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B4" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C4" s="2"/>
-      <x:c r="D4" s="2"/>
-    </x:row>
-    <x:row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B5" s="3"/>
-      <x:c r="C5" s="3"/>
-      <x:c r="D5" s="3"/>
-    </x:row>
-    <x:row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B6" s="1" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C6" s="1"/>
-      <x:c r="D6" s="1"/>
-    </x:row>
-    <x:row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B7" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C7" s="1"/>
-      <x:c r="D7" s="1"/>
-    </x:row>
-    <x:row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B8" s="4"/>
-      <x:c r="C8" s="4"/>
-      <x:c r="D8" s="4"/>
-    </x:row>
-    <x:row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B9" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C9" s="5" t="s">
+      <x:c r="F9" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D9" s="5" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <x:c r="B10" s="5"/>
-      <x:c r="C10" s="5"/>
-      <x:c r="D10" s="5"/>
+    </x:row>
+    <x:row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <x:c r="B10" s="1"/>
+      <x:c r="C10" s="1"/>
+      <x:c r="D10" s="1"/>
+      <x:c r="E10" s="4"/>
+      <x:c r="F10" s="1"/>
     </x:row>
     <x:row r="11">
       <x:c r="B11" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="B12" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="B13" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="B14" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="B15" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C15" t="n">
-        <x:v>27</x:v>
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C15" t="s">
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D15" t="n">
-        <x:v>4454.73</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E15" t="n">
+        <x:v>164.99</x:v>
+      </x:c>
+      <x:c r="F15" t="n">
+        <x:v>659.96</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="B16" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C16" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E16" t="n">
+        <x:v>39.99</x:v>
+      </x:c>
+      <x:c r="F16" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="B17" t="s">
-        <x:v>16</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="B18" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="B19" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="B20" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C20" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D20" t="n">
-        <x:v>329.98</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
       <x:c r="B21" t="s">
-        <x:v>19</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="22">
       <x:c r="B22" t="s">
-        <x:v>20</x:v>
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C22" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D22" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E22" t="n">
+        <x:v>164.99</x:v>
+      </x:c>
+      <x:c r="F22" t="n">
+        <x:v>329.98</x:v>
       </x:c>
     </x:row>
     <x:row r="23">
       <x:c r="B23" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="24">
       <x:c r="B24" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="25">
       <x:c r="B25" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="26">
       <x:c r="B26" t="s">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="27">
       <x:c r="B27" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="28">
       <x:c r="B28" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="29">
       <x:c r="B29" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="30">
       <x:c r="B30" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="31">
       <x:c r="B31" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="32">
       <x:c r="B32" t="s">
-        <x:v>30</x:v>
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C32" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D32" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E32" t="n">
+        <x:v>826.53</x:v>
+      </x:c>
+      <x:c r="F32" t="n">
+        <x:v>826.53</x:v>
       </x:c>
     </x:row>
     <x:row r="33">
       <x:c r="B33" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="34">
       <x:c r="B34" t="s">
-        <x:v>32</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="35">
       <x:c r="B35" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="36">
       <x:c r="B36" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="37">
       <x:c r="B37" t="s">
-        <x:v>35</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="38">
       <x:c r="B38" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
       <x:c r="B39" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C39" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D39" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E39" t="n">
+        <x:v>96.4</x:v>
+      </x:c>
+      <x:c r="F39" t="n">
+        <x:v>192.8</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
       <x:c r="B40" t="s">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="41">
       <x:c r="B41" t="s">
-        <x:v>39</x:v>
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C41" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D41" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E41" t="n">
+        <x:v>720.34</x:v>
+      </x:c>
+      <x:c r="F41" t="n">
+        <x:v>2161.02</x:v>
       </x:c>
     </x:row>
     <x:row r="42">
       <x:c r="B42" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="43">
       <x:c r="B43" t="s">
-        <x:v>41</x:v>
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C43" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D43" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E43" t="n">
+        <x:v>980.1</x:v>
+      </x:c>
+      <x:c r="F43" t="n">
+        <x:v>980.1</x:v>
       </x:c>
     </x:row>
     <x:row r="44">
       <x:c r="B44" t="s">
-        <x:v>42</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="45">
       <x:c r="B45" t="s">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="46">
       <x:c r="B46" t="s">
-        <x:v>44</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="47">
       <x:c r="B47" t="s">
-        <x:v>45</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="48">
       <x:c r="B48" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="49">
       <x:c r="B49" t="s">
-        <x:v>47</x:v>
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50">
+      <x:c r="B50" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51">
+      <x:c r="B51" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52">
+      <x:c r="B52" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53">
+      <x:c r="B53" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54">
+      <x:c r="B54" t="s">
+        <x:v>56</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55">
+      <x:c r="B55" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56">
+      <x:c r="B56" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D56" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="F56" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57">
+      <x:c r="B57" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58">
+      <x:c r="B58" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C58" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D58" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E58" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F58" t="n">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59">
+      <x:c r="B59" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D59" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="F59" t="s">
+        <x:v>64</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="10">
-    <x:mergeCell ref="B8:D8"/>
+  <x:mergeCells count="12">
+    <x:mergeCell ref="B2:F2"/>
+    <x:mergeCell ref="B3:F3"/>
+    <x:mergeCell ref="B4:F4"/>
+    <x:mergeCell ref="B5:F5"/>
+    <x:mergeCell ref="B8:F8"/>
     <x:mergeCell ref="B9:B10"/>
+    <x:mergeCell ref="D9:D10"/>
+    <x:mergeCell ref="F9:F10"/>
+    <x:mergeCell ref="B6:F6"/>
+    <x:mergeCell ref="B7:F7"/>
+    <x:mergeCell ref="E9:E10"/>
     <x:mergeCell ref="C9:C10"/>
-    <x:mergeCell ref="D9:D10"/>
-    <x:mergeCell ref="B6:D6"/>
-    <x:mergeCell ref="B7:D7"/>
-    <x:mergeCell ref="B2:D2"/>
-    <x:mergeCell ref="B3:D3"/>
-    <x:mergeCell ref="B4:D4"/>
-    <x:mergeCell ref="B5:D5"/>
   </x:mergeCells>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Version 2-8-17 Finalizado filtro Clases de Material
</commit_message>
<xml_diff>
--- a/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
+++ b/AppV2/App_Data/reportes/consultor3/ReporteGeneralGastoCapital.xlsx
@@ -53,163 +53,226 @@
     <x:t>FORMULACION PRESUPUESTAL - 2019</x:t>
   </x:si>
   <x:si>
-    <x:t>1.- Materiales y suministros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.- PROGRAMA DE INVERSIONES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.1.- PROYECTOS DE INVERSION PUBLICA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.1.1.- EQUIPAMIENTO E IMPLEMENTACION </x:t>
-  </x:si>
-  <x:si>
-    <x:t>0503280508 - HOJA DE SIERRA DE  2"     X 24" X  6 DIENTES</x:t>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PROGRAMA DE INVERSIONES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PROYECTOS DE INVERSION PUBLICA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPAMIENTO E IMPLEMENTACION </x:t>
+  </x:si>
+  <x:si>
+    <x:t>5505082513 - VALVULA COMPUERTA BRONCE 1.1/4 X 125 LBS P/R</x:t>
+  </x:si>
+  <x:si>
+    <x:t>400716</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GASTOS DE CAPITAL NO LIGADOS A PROYECTOS DE INVERSIÓN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ACTIVOS FIJOS ADMINISTRATIVOS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CENTRO DE COMPUTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.1.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HARDWARE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0476024059 - BOCINA BRONCE SAE 62 5.1/2 X  7.1/2 X  5.1/2" X 16"</x:t>
   </x:si>
   <x:si>
     <x:t>400145</x:t>
   </x:si>
   <x:si>
-    <x:t>5505082513 - VALVULA COMPUERTA BRONCE 1.1/4 X 125 LBS P/R</x:t>
-  </x:si>
-  <x:si>
-    <x:t>400716</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.- GASTOS DE CAPITAL NO LIGADOS A PROYECTOS DE INVERSIÓN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.- ACTIVOS FIJOS ADMINISTRATIVOS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.- CENTRO DE COMPUTO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.1.- HARDWARE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ti</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.2.- SOFTWARE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.2.- desarrollo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.3.- SEGURIDAD DE LA INFORMACIÓN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.4.- CAPACITACIÓN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.1.5.- OTROS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.- EQUIPOS DE INFORMÁTICA Y COMUNICACIONES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.1.- HARDWARE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.2.- SOFTWARE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.2.1.- DESARROLLO</x:t>
+    <x:t>1.2.1.1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOFTWARE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEGURIDAD DE LA INFORMACIÓN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.1.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAPACITACIÓN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.1.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OTROS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPOS DE INFORMÁTICA Y COMUNICACIONES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DESARROLLO</x:t>
   </x:si>
   <x:si>
     <x:t>0341281723 - SOFTWARE SWREUSER V.2.0</x:t>
   </x:si>
   <x:si>
-    <x:t>1.2.1.2.2.2.- DISEÑO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.2.3.- OFIMÁTICA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.2.4.- OTROS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.2.3.- EQUIPO DE COMUNICACIONES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.3.- EQUIPOS DE OFICINA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.3.1.- ADQUISICIÓN EQUIPOS</x:t>
+    <x:t>1.2.1.2.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DISEÑO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OFIMÁTICA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.2.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPO DE COMUNICACIONES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPOS DE OFICINA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ADQUISICIÓN EQUIPOS</x:t>
   </x:si>
   <x:si>
     <x:t>6601011730 - VENTILADOR DE PEDESTAL OSCILANTE</x:t>
   </x:si>
   <x:si>
-    <x:t>1.2.1.3.2.- REPOSICIÓN MOBILIARIO</x:t>
+    <x:t>1.2.1.3.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REPOSICIÓN MOBILIARIO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0503280508 - HOJA DE SIERRA DE  2"     X 24" X  6 DIENTES   </x:t>
   </x:si>
   <x:si>
     <x:t>7460071317 - ESCRITORIO EN MELAMINE EN L DE 1.50 X 1.50 MT GRAFITO C/NEGRO</x:t>
   </x:si>
   <x:si>
-    <x:t>1.2.1.3.3.- OTROS</x:t>
+    <x:t>1.2.1.3.3</x:t>
   </x:si>
   <x:si>
     <x:t>6805131381 - CARRETILLA HIDRAULICA DE 2 TN CAPACIDAD</x:t>
   </x:si>
   <x:si>
-    <x:t>1.2.1.4.- INFRAESTRUCTURA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.1.5.- REPOSICIÓN EQUIPOS DE TRANSPORTE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.- REPOSICIÓN DE ACTIVOS DE PRODUCCIÓN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.1.- MÁQUINAS, EQUIPOS Y HERRAMIENTAS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.2.- EQUIPOS DE CONTROL DE CALIDAD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.3.- INFRAESTRUCTURA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.4.- EQUIPAMIENTO DE TALLERES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.2.5.- OTROS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.3.- PROGRAMA DE ADECUACIÓN MEDIO AMBIENTAL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.3.1.- Gasto Operativo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.3.2.- Implementación</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.2.3.3.- SERVICIOS GESTIÓN INTEGRADA</x:t>
+    <x:t>1.2.1.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INFRAESTRUCTURA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.1.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REPOSICIÓN EQUIPOS DE TRANSPORTE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>REPOSICIÓN DE ACTIVOS DE PRODUCCIÓN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MÁQUINAS, EQUIPOS Y HERRAMIENTAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPOS DE CONTROL DE CALIDAD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EQUIPAMIENTO DE TALLERES</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.2.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PROGRAMA DE ADECUACIÓN MEDIO AMBIENTAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.3.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gasto Operativo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.3.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Implementación</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.2.3.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SERVICIOS GESTIÓN INTEGRADA</x:t>
   </x:si>
   <x:si>
     <x:t>Total Materiales</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5150.39</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2.- Servicios</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SR50343033 - MANIOBRA DE DESMONT. MOTOR PRINCP SALA MAQUNA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total Servicios</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -728,356 +791,413 @@
       <x:c r="F10" s="1"/>
     </x:row>
     <x:row r="11">
+      <x:c r="A11" t="s">
+        <x:v>12</x:v>
+      </x:c>
       <x:c r="B11" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
+      <x:c r="A12" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="B12" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
+      <x:c r="A13" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="B13" t="s">
-        <x:v>14</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="B14" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C14" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D14" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E14" t="n">
+        <x:v>39.99</x:v>
+      </x:c>
+      <x:c r="F14" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
+      <x:c r="A15" t="s">
+        <x:v>20</x:v>
+      </x:c>
       <x:c r="B15" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C15" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D15" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="E15" t="n">
-        <x:v>164.99</x:v>
-      </x:c>
-      <x:c r="F15" t="n">
-        <x:v>659.96</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
+      <x:c r="A16" t="s">
+        <x:v>22</x:v>
+      </x:c>
       <x:c r="B16" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="C16" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D16" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E16" t="n">
-        <x:v>39.99</x:v>
-      </x:c>
-      <x:c r="F16" t="n">
-        <x:v>0</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
+      <x:c r="A17" t="s">
+        <x:v>24</x:v>
+      </x:c>
       <x:c r="B17" t="s">
-        <x:v>20</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
+      <x:c r="A18" t="s">
+        <x:v>26</x:v>
+      </x:c>
       <x:c r="B18" t="s">
-        <x:v>21</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="B19" t="s">
-        <x:v>22</x:v>
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C19" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D19" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E19" t="n">
+        <x:v>1584.93</x:v>
+      </x:c>
+      <x:c r="F19" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
+      <x:c r="A20" t="s">
+        <x:v>30</x:v>
+      </x:c>
       <x:c r="B20" t="s">
-        <x:v>23</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
+      <x:c r="A21" t="s">
+        <x:v>32</x:v>
+      </x:c>
       <x:c r="B21" t="s">
-        <x:v>24</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="22">
+      <x:c r="A22" t="s">
+        <x:v>34</x:v>
+      </x:c>
       <x:c r="B22" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C22" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D22" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E22" t="n">
-        <x:v>164.99</x:v>
-      </x:c>
-      <x:c r="F22" t="n">
-        <x:v>329.98</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="23">
+      <x:c r="A23" t="s">
+        <x:v>36</x:v>
+      </x:c>
       <x:c r="B23" t="s">
-        <x:v>25</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="24">
+      <x:c r="A24" t="s">
+        <x:v>38</x:v>
+      </x:c>
       <x:c r="B24" t="s">
-        <x:v>26</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="25">
+      <x:c r="A25" t="s">
+        <x:v>40</x:v>
+      </x:c>
       <x:c r="B25" t="s">
         <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="26">
+      <x:c r="A26" t="s">
+        <x:v>41</x:v>
+      </x:c>
       <x:c r="B26" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="27">
+      <x:c r="A27" t="s">
+        <x:v>42</x:v>
+      </x:c>
       <x:c r="B27" t="s">
-        <x:v>29</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="28">
       <x:c r="B28" t="s">
-        <x:v>30</x:v>
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C28" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D28" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E28" t="n">
+        <x:v>826.53</x:v>
+      </x:c>
+      <x:c r="F28" t="n">
+        <x:v>826.53</x:v>
       </x:c>
     </x:row>
     <x:row r="29">
+      <x:c r="A29" t="s">
+        <x:v>45</x:v>
+      </x:c>
       <x:c r="B29" t="s">
-        <x:v>31</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="30">
+      <x:c r="A30" t="s">
+        <x:v>47</x:v>
+      </x:c>
       <x:c r="B30" t="s">
-        <x:v>32</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="31">
+      <x:c r="A31" t="s">
+        <x:v>49</x:v>
+      </x:c>
       <x:c r="B31" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="32">
+      <x:c r="A32" t="s">
+        <x:v>50</x:v>
+      </x:c>
       <x:c r="B32" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C32" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D32" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E32" t="n">
-        <x:v>826.53</x:v>
-      </x:c>
-      <x:c r="F32" t="n">
-        <x:v>826.53</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="33">
+      <x:c r="A33" t="s">
+        <x:v>52</x:v>
+      </x:c>
       <x:c r="B33" t="s">
-        <x:v>35</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="34">
+      <x:c r="A34" t="s">
+        <x:v>54</x:v>
+      </x:c>
       <x:c r="B34" t="s">
-        <x:v>36</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
     <x:row r="35">
       <x:c r="B35" t="s">
-        <x:v>37</x:v>
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C35" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D35" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E35" t="n">
+        <x:v>96.4</x:v>
+      </x:c>
+      <x:c r="F35" t="n">
+        <x:v>192.8</x:v>
       </x:c>
     </x:row>
     <x:row r="36">
+      <x:c r="A36" t="s">
+        <x:v>57</x:v>
+      </x:c>
       <x:c r="B36" t="s">
-        <x:v>38</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="37">
       <x:c r="B37" t="s">
-        <x:v>39</x:v>
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C37" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D37" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E37" t="n">
+        <x:v>164.99</x:v>
+      </x:c>
+      <x:c r="F37" t="n">
+        <x:v>989.94</x:v>
       </x:c>
     </x:row>
     <x:row r="38">
       <x:c r="B38" t="s">
-        <x:v>40</x:v>
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C38" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D38" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E38" t="n">
+        <x:v>720.34</x:v>
+      </x:c>
+      <x:c r="F38" t="n">
+        <x:v>2161.02</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
+      <x:c r="A39" t="s">
+        <x:v>61</x:v>
+      </x:c>
       <x:c r="B39" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C39" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D39" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E39" t="n">
-        <x:v>96.4</x:v>
-      </x:c>
-      <x:c r="F39" t="n">
-        <x:v>192.8</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
       <x:c r="B40" t="s">
-        <x:v>42</x:v>
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C40" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D40" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E40" t="n">
+        <x:v>980.1</x:v>
+      </x:c>
+      <x:c r="F40" t="n">
+        <x:v>980.1</x:v>
       </x:c>
     </x:row>
     <x:row r="41">
+      <x:c r="A41" t="s">
+        <x:v>63</x:v>
+      </x:c>
       <x:c r="B41" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C41" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D41" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E41" t="n">
-        <x:v>720.34</x:v>
-      </x:c>
-      <x:c r="F41" t="n">
-        <x:v>2161.02</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="42">
+      <x:c r="A42" t="s">
+        <x:v>65</x:v>
+      </x:c>
       <x:c r="B42" t="s">
-        <x:v>44</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="43">
+      <x:c r="A43" t="s">
+        <x:v>67</x:v>
+      </x:c>
       <x:c r="B43" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C43" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D43" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E43" t="n">
-        <x:v>980.1</x:v>
-      </x:c>
-      <x:c r="F43" t="n">
-        <x:v>980.1</x:v>
+        <x:v>68</x:v>
       </x:c>
     </x:row>
     <x:row r="44">
+      <x:c r="A44" t="s">
+        <x:v>69</x:v>
+      </x:c>
       <x:c r="B44" t="s">
-        <x:v>46</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="45">
+      <x:c r="A45" t="s">
+        <x:v>71</x:v>
+      </x:c>
       <x:c r="B45" t="s">
-        <x:v>47</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="46">
+      <x:c r="A46" t="s">
+        <x:v>73</x:v>
+      </x:c>
       <x:c r="B46" t="s">
-        <x:v>48</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="47">
+      <x:c r="A47" t="s">
+        <x:v>74</x:v>
+      </x:c>
       <x:c r="B47" t="s">
-        <x:v>49</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="48">
+      <x:c r="A48" t="s">
+        <x:v>76</x:v>
+      </x:c>
       <x:c r="B48" t="s">
-        <x:v>50</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="49">
+      <x:c r="A49" t="s">
+        <x:v>77</x:v>
+      </x:c>
       <x:c r="B49" t="s">
-        <x:v>51</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="50">
+      <x:c r="A50" t="s">
+        <x:v>79</x:v>
+      </x:c>
       <x:c r="B50" t="s">
-        <x:v>52</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="51">
+      <x:c r="A51" t="s">
+        <x:v>81</x:v>
+      </x:c>
       <x:c r="B51" t="s">
-        <x:v>53</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="52">
+      <x:c r="A52" t="s">
+        <x:v>83</x:v>
+      </x:c>
       <x:c r="B52" t="s">
-        <x:v>54</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="53">
       <x:c r="B53" t="s">
-        <x:v>55</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54">
-      <x:c r="B54" t="s">
-        <x:v>56</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55">
-      <x:c r="B55" t="s">
-        <x:v>57</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56">
-      <x:c r="B56" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="D56" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="F56" t="s">
-        <x:v>60</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57">
-      <x:c r="B57" t="s">
-        <x:v>61</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58">
-      <x:c r="B58" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="C58" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D58" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E58" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F58" t="n">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59">
-      <x:c r="B59" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="D59" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="F59" t="s">
-        <x:v>64</x:v>
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D53" t="n">
+        <x:v>13.00</x:v>
+      </x:c>
+      <x:c r="F53" t="n">
+        <x:v>5150.39</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>